<commit_message>
Se agrega Alumno 5 al archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SCRProteus\ISPC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SCRProteus\ISPC\Alumnos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB78A7C-5E7A-4275-93EA-07A0678A2D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F883D7-498F-409A-B064-3C048C842CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>#</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t>alfredo.pc@gmail.com</t>
+  </si>
+  <si>
+    <t>Leonardo Gonzalez</t>
+  </si>
+  <si>
+    <t>leogb37@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -422,7 +428,7 @@
   <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -523,9 +529,15 @@
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4">
+        <v>2</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1020,8 +1032,9 @@
     <hyperlink ref="D3" r:id="rId2" xr:uid="{6B0894EE-ABAA-4E3D-B4DD-0AE31FFED46A}"/>
     <hyperlink ref="D4" r:id="rId3" xr:uid="{A9805738-DF32-489E-91F7-DF462DDF76CD}"/>
     <hyperlink ref="D5" r:id="rId4" xr:uid="{8770EE02-9DB0-4D05-ADA7-E46BB0180097}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{BC2315A1-41FD-452A-BAEC-35F349BE3512}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega la 6 Alumna
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SCRProteus\ISPC\Alumnos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F883D7-498F-409A-B064-3C048C842CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7333D2-46F7-4D3F-A458-75AD81B70993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>#</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>leogb37@gmail.com</t>
+  </si>
+  <si>
+    <t>Lorena Milianovich</t>
+  </si>
+  <si>
+    <t>lmilianovich@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -428,7 +434,7 @@
   <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -544,9 +550,15 @@
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="4">
+        <v>4</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1033,8 +1045,9 @@
     <hyperlink ref="D4" r:id="rId3" xr:uid="{A9805738-DF32-489E-91F7-DF462DDF76CD}"/>
     <hyperlink ref="D5" r:id="rId4" xr:uid="{8770EE02-9DB0-4D05-ADA7-E46BB0180097}"/>
     <hyperlink ref="D6" r:id="rId5" xr:uid="{BC2315A1-41FD-452A-BAEC-35F349BE3512}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{28B5A7B0-A616-4CA3-B679-3281575599AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega el 7 Alumno
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SCRProteus\ISPC\Alumnos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7333D2-46F7-4D3F-A458-75AD81B70993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5550530D-8D8D-4843-8F26-B335D492B768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>#</t>
   </si>
@@ -77,6 +77,15 @@
   </si>
   <si>
     <t>lmilianovich@gmail.com</t>
+  </si>
+  <si>
+    <t>Juan Diego Gonzalez Antoniazzi</t>
+  </si>
+  <si>
+    <t>jdgaprogrammer@gmail.com</t>
+  </si>
+  <si>
+    <t>jdga1997</t>
   </si>
 </sst>
 </file>
@@ -434,7 +443,7 @@
   <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -565,10 +574,18 @@
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="4">
+        <v>3</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
@@ -1046,8 +1063,9 @@
     <hyperlink ref="D5" r:id="rId4" xr:uid="{8770EE02-9DB0-4D05-ADA7-E46BB0180097}"/>
     <hyperlink ref="D6" r:id="rId5" xr:uid="{BC2315A1-41FD-452A-BAEC-35F349BE3512}"/>
     <hyperlink ref="D7" r:id="rId6" xr:uid="{28B5A7B0-A616-4CA3-B679-3281575599AD}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{EBC42CBC-B2DC-4299-9921-7B46D2884027}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega la 8 Alumna
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SCRProteus\ISPC\Alumnos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5550530D-8D8D-4843-8F26-B335D492B768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77045E63-8268-4710-A31F-287DD1B8B225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>#</t>
   </si>
@@ -86,6 +86,15 @@
   </si>
   <si>
     <t>jdga1997</t>
+  </si>
+  <si>
+    <t>Natalia Galliani</t>
+  </si>
+  <si>
+    <t>gallianinatalia@gmail.com</t>
+  </si>
+  <si>
+    <t>NataliaGalliani</t>
   </si>
 </sst>
 </file>
@@ -443,7 +452,7 @@
   <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -591,10 +600,18 @@
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="4">
+        <v>3</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
@@ -1064,8 +1081,9 @@
     <hyperlink ref="D6" r:id="rId5" xr:uid="{BC2315A1-41FD-452A-BAEC-35F349BE3512}"/>
     <hyperlink ref="D7" r:id="rId6" xr:uid="{28B5A7B0-A616-4CA3-B679-3281575599AD}"/>
     <hyperlink ref="D8" r:id="rId7" xr:uid="{EBC42CBC-B2DC-4299-9921-7B46D2884027}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{FF05B8F9-5443-4067-8422-A2110A7969CD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega alumno no valido
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SCRProteus\ISPC\Alumnos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77045E63-8268-4710-A31F-287DD1B8B225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58CE7F6-FEA2-4C12-8555-8911CBA274F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>#</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t>NataliaGalliani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juan Perez </t>
+  </si>
+  <si>
+    <t>dire@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -452,7 +458,7 @@
   <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -617,10 +623,18 @@
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
@@ -1082,8 +1096,9 @@
     <hyperlink ref="D7" r:id="rId6" xr:uid="{28B5A7B0-A616-4CA3-B679-3281575599AD}"/>
     <hyperlink ref="D8" r:id="rId7" xr:uid="{EBC42CBC-B2DC-4299-9921-7B46D2884027}"/>
     <hyperlink ref="D9" r:id="rId8" xr:uid="{FF05B8F9-5443-4067-8422-A2110A7969CD}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{D05A7570-2927-40F3-B2AA-31347FA71425}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se crea la lista de alumnos
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SCRProteus\ISPC\Alumnos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58CE7F6-FEA2-4C12-8555-8911CBA274F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDC5557-EC19-4FAE-97A0-F6E71752FD0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>#</t>
   </si>
@@ -35,72 +35,6 @@
   </si>
   <si>
     <t>nombre github</t>
-  </si>
-  <si>
-    <t>advanceezequiel@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ezequiel Mansilla </t>
-  </si>
-  <si>
-    <t>Ezequiel Manzilla</t>
-  </si>
-  <si>
-    <t>Cristian Cabañas</t>
-  </si>
-  <si>
-    <t>ccristianjc@gmail.com</t>
-  </si>
-  <si>
-    <t>Sergio Muguruza</t>
-  </si>
-  <si>
-    <t>sergiomuguruza@gmail.com</t>
-  </si>
-  <si>
-    <t>Sergio muguruza</t>
-  </si>
-  <si>
-    <t>Alfredo Palacios</t>
-  </si>
-  <si>
-    <t>alfredo.pc@gmail.com</t>
-  </si>
-  <si>
-    <t>Leonardo Gonzalez</t>
-  </si>
-  <si>
-    <t>leogb37@gmail.com</t>
-  </si>
-  <si>
-    <t>Lorena Milianovich</t>
-  </si>
-  <si>
-    <t>lmilianovich@gmail.com</t>
-  </si>
-  <si>
-    <t>Juan Diego Gonzalez Antoniazzi</t>
-  </si>
-  <si>
-    <t>jdgaprogrammer@gmail.com</t>
-  </si>
-  <si>
-    <t>jdga1997</t>
-  </si>
-  <si>
-    <t>Natalia Galliani</t>
-  </si>
-  <si>
-    <t>gallianinatalia@gmail.com</t>
-  </si>
-  <si>
-    <t>NataliaGalliani</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Juan Perez </t>
-  </si>
-  <si>
-    <t>dire@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -458,7 +392,7 @@
   <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -491,150 +425,82 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4">
-        <v>4</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="4">
-        <v>2</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="4">
-        <v>2</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="4">
-        <v>4</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>18</v>
-      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="4">
-        <v>3</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="4">
-        <v>3</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
@@ -1087,18 +953,7 @@
       <c r="E60" s="4"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{DEAF24B4-68F4-4818-AF58-13F0F00F56F7}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{6B0894EE-ABAA-4E3D-B4DD-0AE31FFED46A}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{A9805738-DF32-489E-91F7-DF462DDF76CD}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{8770EE02-9DB0-4D05-ADA7-E46BB0180097}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{BC2315A1-41FD-452A-BAEC-35F349BE3512}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{28B5A7B0-A616-4CA3-B679-3281575599AD}"/>
-    <hyperlink ref="D8" r:id="rId7" xr:uid="{EBC42CBC-B2DC-4299-9921-7B46D2884027}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{FF05B8F9-5443-4067-8422-A2110A7969CD}"/>
-    <hyperlink ref="D10" r:id="rId9" xr:uid="{D05A7570-2927-40F3-B2AA-31347FA71425}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Agrego mis datos a Lista de Alumnos.xlsx
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4506"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SCRProteus\ISPC\Alumnos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDC5557-EC19-4FAE-97A0-F6E71752FD0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Electronica Microcontrolada" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>#</t>
   </si>
@@ -36,12 +30,21 @@
   <si>
     <t>nombre github</t>
   </si>
+  <si>
+    <t>Natalia A. Galliani</t>
+  </si>
+  <si>
+    <t>gallianinatalia@gmail.com</t>
+  </si>
+  <si>
+    <t>NataliaGalliani</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -385,17 +388,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="6.85546875" customWidth="1"/>
     <col min="2" max="2" width="37.140625" customWidth="1"/>
@@ -404,7 +407,7 @@
     <col min="5" max="5" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="32.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -421,16 +424,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="25.5" customHeight="1">
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="25.5" customHeight="1">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -439,7 +450,7 @@
       <c r="D3" s="5"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="25.5" customHeight="1">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -448,7 +459,7 @@
       <c r="D4" s="6"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="25.5" customHeight="1">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -457,7 +468,7 @@
       <c r="D5" s="6"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="25.5" customHeight="1">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -466,7 +477,7 @@
       <c r="D6" s="6"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="25.5" customHeight="1">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -475,7 +486,7 @@
       <c r="D7" s="6"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="25.5" customHeight="1">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -484,7 +495,7 @@
       <c r="D8" s="6"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="25.5" customHeight="1">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -493,7 +504,7 @@
       <c r="D9" s="6"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="25.5" customHeight="1">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -502,7 +513,7 @@
       <c r="D10" s="6"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="25.5" customHeight="1">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -511,7 +522,7 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="25.5" customHeight="1">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -520,7 +531,7 @@
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="25.5" customHeight="1">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -529,7 +540,7 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="25.5" customHeight="1">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -538,7 +549,7 @@
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="25.5" customHeight="1">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -547,7 +558,7 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="25.5" customHeight="1">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -556,7 +567,7 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="25.5" customHeight="1">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -565,7 +576,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="25.5" customHeight="1">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -574,7 +585,7 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="25.5" customHeight="1">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -583,7 +594,7 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="25.5" customHeight="1">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -592,7 +603,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="25.5" customHeight="1">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -601,7 +612,7 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="25.5" customHeight="1">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -610,7 +621,7 @@
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="25.5" customHeight="1">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -619,7 +630,7 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="25.5" customHeight="1">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -628,7 +639,7 @@
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="25.5" customHeight="1">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -637,7 +648,7 @@
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="25.5" customHeight="1">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -646,7 +657,7 @@
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="25.5" customHeight="1">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -655,7 +666,7 @@
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="25.5" customHeight="1">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -664,7 +675,7 @@
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="25.5" customHeight="1">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -673,7 +684,7 @@
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="25.5" customHeight="1">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -682,7 +693,7 @@
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="25.5" customHeight="1">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -691,7 +702,7 @@
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="25.5" customHeight="1">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -700,7 +711,7 @@
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="25.5" customHeight="1">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -709,7 +720,7 @@
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="25.5" customHeight="1">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -718,7 +729,7 @@
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
     </row>
-    <row r="35" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="25.5" customHeight="1">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -727,7 +738,7 @@
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="25.5" customHeight="1">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -736,7 +747,7 @@
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
     </row>
-    <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="25.5" customHeight="1">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -745,7 +756,7 @@
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
     </row>
-    <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="25.5" customHeight="1">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -754,7 +765,7 @@
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
     </row>
-    <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="25.5" customHeight="1">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -763,7 +774,7 @@
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
     </row>
-    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="25.5" customHeight="1">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -772,7 +783,7 @@
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
     </row>
-    <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="25.5" customHeight="1">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -781,7 +792,7 @@
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
     </row>
-    <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="25.5" customHeight="1">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -790,7 +801,7 @@
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
     </row>
-    <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="25.5" customHeight="1">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -799,7 +810,7 @@
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
     </row>
-    <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="25.5" customHeight="1">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -808,7 +819,7 @@
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
     </row>
-    <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="25.5" customHeight="1">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -817,7 +828,7 @@
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
     </row>
-    <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="25.5" customHeight="1">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -826,7 +837,7 @@
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
     </row>
-    <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="25.5" customHeight="1">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -835,7 +846,7 @@
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
     </row>
-    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="25.5" customHeight="1">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -844,7 +855,7 @@
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
     </row>
-    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="25.5" customHeight="1">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -853,7 +864,7 @@
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
     </row>
-    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="25.5" customHeight="1">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -862,7 +873,7 @@
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
     </row>
-    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="25.5" customHeight="1">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -871,7 +882,7 @@
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
     </row>
-    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="25.5" customHeight="1">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -880,7 +891,7 @@
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
     </row>
-    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="25.5" customHeight="1">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -889,7 +900,7 @@
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
     </row>
-    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" ht="25.5" customHeight="1">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -898,7 +909,7 @@
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
     </row>
-    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" ht="25.5" customHeight="1">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -907,7 +918,7 @@
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
     </row>
-    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" ht="25.5" customHeight="1">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -916,7 +927,7 @@
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
     </row>
-    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" ht="25.5" customHeight="1">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -925,7 +936,7 @@
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
     </row>
-    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" ht="25.5" customHeight="1">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -934,7 +945,7 @@
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
     </row>
-    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" ht="25.5" customHeight="1">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -943,7 +954,7 @@
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
     </row>
-    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" ht="25.5" customHeight="1">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -953,7 +964,10 @@
       <c r="E60" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega el 4 Alumno al archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roxana Vicentelo\Documents\ispc\electronica\semana 2\repo\Alumnos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF99A3A8-0498-4932-8ED0-1ECE6A14C969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Electronica Microcontrolada" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Electronica Microcontrolada" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -20,77 +25,67 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t xml:space="preserve">#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre y Apellido</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aula</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nombre github</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Natalia A. Galliani</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gallianinatalia@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NataliaGalliani</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gustavo Alberto Godoy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gustavogodoy85@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rebeca Ruth Veronica Morales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">morales-rebeca@hotmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rebmorales</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Nombre y Apellido</t>
+  </si>
+  <si>
+    <t>Aula</t>
+  </si>
+  <si>
+    <t>mail</t>
+  </si>
+  <si>
+    <t>nombre github</t>
+  </si>
+  <si>
+    <t>Natalia A. Galliani</t>
+  </si>
+  <si>
+    <t>gallianinatalia@gmail.com</t>
+  </si>
+  <si>
+    <t>NataliaGalliani</t>
+  </si>
+  <si>
+    <t>Gustavo Alberto Godoy</t>
+  </si>
+  <si>
+    <t>gustavogodoy85@gmail.com</t>
+  </si>
+  <si>
+    <t>Rebeca Ruth Veronica Morales</t>
+  </si>
+  <si>
+    <t>morales-rebeca@hotmail.com</t>
+  </si>
+  <si>
+    <t>rebmorales</t>
+  </si>
+  <si>
+    <t>Roxana Abigail Vicentelo</t>
+  </si>
+  <si>
+    <t>abigailvicentelo@gmail.com</t>
+  </si>
+  <si>
+    <t>vicenteloroxana</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="18"/>
@@ -107,7 +102,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -115,10 +110,18 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -132,146 +135,437 @@
     </fill>
   </fills>
   <borders count="5">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="37.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="31.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="29.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
+    <col min="1" max="1" width="6.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31" style="2" customWidth="1"/>
+    <col min="5" max="5" width="29" style="2" customWidth="1"/>
+    <col min="6" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -288,14 +582,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="n">
+    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7" t="n">
+      <c r="C2" s="7">
         <v>3</v>
       </c>
       <c r="D2" s="9" t="s">
@@ -305,14 +599,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="n">
+    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C3" s="7">
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
@@ -320,14 +614,14 @@
       </c>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="n">
+    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="7" t="n">
+      <c r="C4" s="7">
         <v>4</v>
       </c>
       <c r="D4" s="9" t="s">
@@ -337,17 +631,25 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
+    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
+      <c r="B5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="7">
+        <v>3</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
       <c r="B6" s="8"/>
@@ -355,8 +657,8 @@
       <c r="D6" s="9"/>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="n">
+    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
       <c r="B7" s="8"/>
@@ -364,8 +666,8 @@
       <c r="D7" s="9"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="n">
+    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>7</v>
       </c>
       <c r="B8" s="8"/>
@@ -373,8 +675,8 @@
       <c r="D8" s="9"/>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="n">
+    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
         <v>8</v>
       </c>
       <c r="B9" s="8"/>
@@ -382,8 +684,8 @@
       <c r="D9" s="9"/>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="n">
+    <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <v>9</v>
       </c>
       <c r="B10" s="8"/>
@@ -391,8 +693,8 @@
       <c r="D10" s="9"/>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="n">
+    <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
         <v>10</v>
       </c>
       <c r="B11" s="8"/>
@@ -400,8 +702,8 @@
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="n">
+    <row r="12" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
         <v>11</v>
       </c>
       <c r="B12" s="8"/>
@@ -409,8 +711,8 @@
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="n">
+    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
         <v>12</v>
       </c>
       <c r="B13" s="8"/>
@@ -418,8 +720,8 @@
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="n">
+    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
         <v>13</v>
       </c>
       <c r="B14" s="8"/>
@@ -427,8 +729,8 @@
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="n">
+    <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
         <v>14</v>
       </c>
       <c r="B15" s="8"/>
@@ -436,8 +738,8 @@
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="n">
+    <row r="16" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
         <v>15</v>
       </c>
       <c r="B16" s="8"/>
@@ -445,8 +747,8 @@
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="n">
+    <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
         <v>16</v>
       </c>
       <c r="B17" s="8"/>
@@ -454,8 +756,8 @@
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="n">
+    <row r="18" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
         <v>17</v>
       </c>
       <c r="B18" s="8"/>
@@ -463,8 +765,8 @@
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="n">
+    <row r="19" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
         <v>18</v>
       </c>
       <c r="B19" s="8"/>
@@ -472,8 +774,8 @@
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="n">
+    <row r="20" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
         <v>19</v>
       </c>
       <c r="B20" s="8"/>
@@ -481,8 +783,8 @@
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="n">
+    <row r="21" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
         <v>20</v>
       </c>
       <c r="B21" s="8"/>
@@ -490,8 +792,8 @@
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="n">
+    <row r="22" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
         <v>21</v>
       </c>
       <c r="B22" s="8"/>
@@ -499,8 +801,8 @@
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="n">
+    <row r="23" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
         <v>22</v>
       </c>
       <c r="B23" s="8"/>
@@ -508,8 +810,8 @@
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="n">
+    <row r="24" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
         <v>23</v>
       </c>
       <c r="B24" s="8"/>
@@ -517,8 +819,8 @@
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7" t="n">
+    <row r="25" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
         <v>24</v>
       </c>
       <c r="B25" s="8"/>
@@ -526,8 +828,8 @@
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7" t="n">
+    <row r="26" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
         <v>25</v>
       </c>
       <c r="B26" s="8"/>
@@ -535,8 +837,8 @@
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7" t="n">
+    <row r="27" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
         <v>26</v>
       </c>
       <c r="B27" s="8"/>
@@ -544,8 +846,8 @@
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="n">
+    <row r="28" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
         <v>27</v>
       </c>
       <c r="B28" s="8"/>
@@ -553,8 +855,8 @@
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
     </row>
-    <row r="29" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7" t="n">
+    <row r="29" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
         <v>28</v>
       </c>
       <c r="B29" s="8"/>
@@ -562,8 +864,8 @@
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
     </row>
-    <row r="30" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="n">
+    <row r="30" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
         <v>29</v>
       </c>
       <c r="B30" s="8"/>
@@ -571,8 +873,8 @@
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
     </row>
-    <row r="31" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="n">
+    <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
         <v>30</v>
       </c>
       <c r="B31" s="8"/>
@@ -580,8 +882,8 @@
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7" t="n">
+    <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
         <v>31</v>
       </c>
       <c r="B32" s="8"/>
@@ -589,8 +891,8 @@
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7" t="n">
+    <row r="33" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
         <v>32</v>
       </c>
       <c r="B33" s="8"/>
@@ -598,8 +900,8 @@
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
     </row>
-    <row r="34" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7" t="n">
+    <row r="34" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
         <v>33</v>
       </c>
       <c r="B34" s="8"/>
@@ -607,8 +909,8 @@
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
     </row>
-    <row r="35" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7" t="n">
+    <row r="35" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
         <v>34</v>
       </c>
       <c r="B35" s="8"/>
@@ -616,8 +918,8 @@
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
     </row>
-    <row r="36" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7" t="n">
+    <row r="36" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
         <v>35</v>
       </c>
       <c r="B36" s="8"/>
@@ -625,8 +927,8 @@
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
     </row>
-    <row r="37" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7" t="n">
+    <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
         <v>36</v>
       </c>
       <c r="B37" s="8"/>
@@ -634,8 +936,8 @@
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
     </row>
-    <row r="38" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7" t="n">
+    <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
         <v>37</v>
       </c>
       <c r="B38" s="8"/>
@@ -643,8 +945,8 @@
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
     </row>
-    <row r="39" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="7" t="n">
+    <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
         <v>38</v>
       </c>
       <c r="B39" s="8"/>
@@ -652,8 +954,8 @@
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
     </row>
-    <row r="40" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7" t="n">
+    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
         <v>39</v>
       </c>
       <c r="B40" s="8"/>
@@ -661,8 +963,8 @@
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
     </row>
-    <row r="41" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="7" t="n">
+    <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
         <v>40</v>
       </c>
       <c r="B41" s="8"/>
@@ -670,8 +972,8 @@
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
     </row>
-    <row r="42" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="7" t="n">
+    <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
         <v>41</v>
       </c>
       <c r="B42" s="8"/>
@@ -679,8 +981,8 @@
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
     </row>
-    <row r="43" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7" t="n">
+    <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
         <v>42</v>
       </c>
       <c r="B43" s="8"/>
@@ -688,8 +990,8 @@
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
     </row>
-    <row r="44" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="7" t="n">
+    <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
         <v>43</v>
       </c>
       <c r="B44" s="8"/>
@@ -697,8 +999,8 @@
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
     </row>
-    <row r="45" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="7" t="n">
+    <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
         <v>44</v>
       </c>
       <c r="B45" s="8"/>
@@ -706,8 +1008,8 @@
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
     </row>
-    <row r="46" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="7" t="n">
+    <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
         <v>45</v>
       </c>
       <c r="B46" s="8"/>
@@ -715,8 +1017,8 @@
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
     </row>
-    <row r="47" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="7" t="n">
+    <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
         <v>46</v>
       </c>
       <c r="B47" s="8"/>
@@ -724,8 +1026,8 @@
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
     </row>
-    <row r="48" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="7" t="n">
+    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="7">
         <v>47</v>
       </c>
       <c r="B48" s="8"/>
@@ -733,8 +1035,8 @@
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
     </row>
-    <row r="49" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="7" t="n">
+    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
         <v>48</v>
       </c>
       <c r="B49" s="8"/>
@@ -742,8 +1044,8 @@
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
     </row>
-    <row r="50" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="7" t="n">
+    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
         <v>49</v>
       </c>
       <c r="B50" s="8"/>
@@ -751,8 +1053,8 @@
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
     </row>
-    <row r="51" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="7" t="n">
+    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
         <v>50</v>
       </c>
       <c r="B51" s="8"/>
@@ -760,8 +1062,8 @@
       <c r="D51" s="8"/>
       <c r="E51" s="8"/>
     </row>
-    <row r="52" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="7" t="n">
+    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
         <v>51</v>
       </c>
       <c r="B52" s="8"/>
@@ -769,8 +1071,8 @@
       <c r="D52" s="8"/>
       <c r="E52" s="8"/>
     </row>
-    <row r="53" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="7" t="n">
+    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="7">
         <v>52</v>
       </c>
       <c r="B53" s="8"/>
@@ -778,8 +1080,8 @@
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
     </row>
-    <row r="54" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="7" t="n">
+    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="7">
         <v>53</v>
       </c>
       <c r="B54" s="8"/>
@@ -787,8 +1089,8 @@
       <c r="D54" s="8"/>
       <c r="E54" s="8"/>
     </row>
-    <row r="55" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="7" t="n">
+    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="7">
         <v>54</v>
       </c>
       <c r="B55" s="8"/>
@@ -796,8 +1098,8 @@
       <c r="D55" s="8"/>
       <c r="E55" s="8"/>
     </row>
-    <row r="56" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="7" t="n">
+    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="7">
         <v>55</v>
       </c>
       <c r="B56" s="8"/>
@@ -805,8 +1107,8 @@
       <c r="D56" s="8"/>
       <c r="E56" s="8"/>
     </row>
-    <row r="57" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="7" t="n">
+    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="7">
         <v>56</v>
       </c>
       <c r="B57" s="8"/>
@@ -814,8 +1116,8 @@
       <c r="D57" s="8"/>
       <c r="E57" s="8"/>
     </row>
-    <row r="58" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="7" t="n">
+    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="7">
         <v>57</v>
       </c>
       <c r="B58" s="8"/>
@@ -823,8 +1125,8 @@
       <c r="D58" s="8"/>
       <c r="E58" s="8"/>
     </row>
-    <row r="59" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="7" t="n">
+    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="7">
         <v>58</v>
       </c>
       <c r="B59" s="8"/>
@@ -832,8 +1134,8 @@
       <c r="D59" s="8"/>
       <c r="E59" s="8"/>
     </row>
-    <row r="60" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="7" t="n">
+    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="7">
         <v>59</v>
       </c>
       <c r="B60" s="8"/>
@@ -843,14 +1145,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" display="morales-rebeca@hotmail.com"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{A75F96B5-6B15-4B66-A61C-A27306CFF847}"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>